<commit_message>
Steady state freq analysis
</commit_message>
<xml_diff>
--- a/scripts_steadystate/proc_notes.xlsx
+++ b/scripts_steadystate/proc_notes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emiljohansen/Documents/Laosdirg/Roskilde/roskilde-eeg-pipeline/data/Nicolet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emiljohansen/Documents/Laosdirg/Roskilde/roskilde-eeg-pipeline/scripts_steadystate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D72A26-4506-A749-B77E-52557DA180FA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FAFE2B-D67A-7648-80F2-EA222D99C960}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="460" windowWidth="27760" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,26 +28,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>subject</t>
   </si>
   <si>
-    <t>oddballidx</t>
-  </si>
-  <si>
-    <t>standardballidx</t>
-  </si>
-  <si>
     <t>data_available</t>
   </si>
   <si>
-    <t>1,900</t>
-  </si>
-  <si>
-    <t>1,100</t>
-  </si>
-  <si>
     <t>s1001</t>
   </si>
   <si>
@@ -96,85 +84,37 @@
     <t>s1016</t>
   </si>
   <si>
-    <t>24, 81, 167, 190, 246, 263, 264, 428, 453, 468, 507, 509, 565, 566, 681, 725, 726, 772, 773, 779, 785, 808, 856, 859</t>
-  </si>
-  <si>
-    <t>bad_trials_standardball</t>
-  </si>
-  <si>
-    <t>bad_trials_oddball</t>
-  </si>
-  <si>
-    <t>4, 5, 13, 34, 63, 80, 95</t>
-  </si>
-  <si>
     <t>bad_channels_standardball</t>
   </si>
   <si>
     <t>bad_channels_oddball</t>
   </si>
   <si>
-    <t>1, 2, 72, 73, 124, 184, 212, 213, 214, 330, 331, 409, 443, 482, 503, 518, 553, 554, 590, 591, 660, 802, 882</t>
-  </si>
-  <si>
-    <t>1, 29, 30, 69, 89, 115, 126, 133, 143, 160, 199, 212, 239, 241, 252, 253, 274, 284, 309, 332, 351, 356, 370, 386, 398, 416, 417, 418, 419, 421, 424, 428, 432, 438, 464, 469, 490, 501, 512, 513, 550, 551, 552, 558, 561, 562, 564, 565, 577, 578, 591, 592, 638, 661, 662, 663, 690, 693, 710, 712, 719, 721, 732, 733, 735, 736, 755, 756, 760, 761, 762, 795, 802, 807, 832, 833, 834, 835, 836, 840, 849, 850, 851, 852, 862, 863, 865, 867, 879, 885, 891, 893, 894</t>
-  </si>
-  <si>
-    <t>27, 33, 54, 57, 63, 78, 81, 97</t>
-  </si>
-  <si>
     <t>Fp1, Fp2, 25</t>
   </si>
   <si>
-    <t>2, 17, 19, 46, 47, 58, 98, 99, 106, 108, 135, 149, 187, 206, 254, 275, 277, 308, 317, 357, 360, 393, 395, 467, 492, 493, 494, 533, 534, 588, 629, 639, 647, 649, 652, 654, 664, 680, 681, 715, 718, 719, 724, 756, 843, 844, 845, 859, 860, 865, 866, 867, 868, 869, 871, 872, 887, 900</t>
-  </si>
-  <si>
-    <t>14, 37, 92, 94, 96</t>
-  </si>
-  <si>
-    <t>4, 9, 10, 11, 12, 13, 14, 15, 16, 20, 21, 28, 33, 97, 129, 134, 137, 149, 208, 236, 239, 254, 256, 260, 261, 262, 263, 264, 266, 269, 271, 290, 291, 292, 293, 305, 325, 326, 327, 330, 365, 366, 368, 380, 391, 392, 475, 482, 499, 506, 510, 579, 603, 605, 607, 610, 611, 613, 640, 641, 681, 761, 781, 782, 788, 790, 799, 801, 802, 803, 804, 805, 806, 808, 811, 837, 839, 840, 841, 842, 843, 844, 845, 848, 870, 879, 888</t>
-  </si>
-  <si>
-    <t>1, 2, 26, 31, 36, 37, 43, 44, 46, 71, 79, 81, 90</t>
-  </si>
-  <si>
-    <t>4,902</t>
-  </si>
-  <si>
-    <t>64, 65, 67, 100, 105, 137, 144, 169, 178, 277, 309, 320, 483, 492, 555, 577, 584, 585, 590, 594, 632, 800, 801, 802, 826, 893</t>
-  </si>
-  <si>
-    <t>31, 40, 57, 62, 67</t>
-  </si>
-  <si>
-    <t>1, 2, 3, 8, 9, 10, 11, 31, 44, 45, 49, 56, 57, 94, 103, 119, 125, 127, 140, 141, 144, 145, 191, 192, 194, 196, 197, 198, 199, 220, 221, 277, 278, 279, 280, 281, 293, 298, 299, 306, 307, 308, 313, 314, 323, 324, 325, 337, 348, 395, 396, 401, 402, 480, 526, 527, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 541, 542, 543, 547, 550, 554, 555, 560, 565, 566, 567, 570, 571, 572, 573, 603, 604, 606, 612, 623, 624, 629, 631, 633, 634, 635, 637, 643, 644, 649, 662, 663, 665, 666, 667, 680, 683, 712, 714, 722, 724, 725, 729, 734, 735, 736, 738, 745, 751, 770, 776, 780, 781, 783, 796, 797, 798, 799, 801, 802, 810, 811, 830, 831, 852, 875, 876, 877, 891, 892</t>
-  </si>
-  <si>
-    <t>7, 24, 38, 56, 60, 61, 62, 63, 69, 74, 81, 83, 93</t>
-  </si>
-  <si>
-    <t>33, 116, 127, 269, 270, 271, 272, 275, 276, 287, 357, 493, 516, 522, 523, 524, 529, 530, 533, 536, 537, 573, 577, 578, 605, 660, 753, 754, 756, 757, 766, 769, 771, 772, 773, 833, 835, 836, 837, 841, 860, 862</t>
-  </si>
-  <si>
-    <t>37, 59, 61, 64, 75, 88, 95, 96</t>
-  </si>
-  <si>
-    <t>18, 86, 87, 154, 197, 199, 358, 367, 429, 430, 449, 480, 542, 543, 584, 604, 616, 693, 757, 785, 806, 829, 832, 833, 834, 835, 840, 842, 871, 872, 873, 875, 883</t>
-  </si>
-  <si>
-    <t>7, 74, 85, 89, 99</t>
-  </si>
-  <si>
-    <t>44, 170, 186, 280, 385, 402, 404, 413, 439, 457, 489, 519, 545, 546, 551, 580, 603, 610, 633, 704, 734, 747, 751, 777, 800, 862</t>
-  </si>
-  <si>
-    <t>59, 79</t>
-  </si>
-  <si>
-    <t>8, 16, 17, 25, 33, 34, 63, 74, 75, 128, 140, 152, 154, 172, 179, 195, 236, 242, 247, 308, 312, 317, 333, 334, 349, 360, 406, 437, 439, 447, 451, 529, 533, 547, 559, 581, 602, 620, 621, 664, 674, 678, 686, 697, 713, 715, 790, 810, 828, 893</t>
-  </si>
-  <si>
-    <t>1, 3, 10, 18, 40, 50, 52, 53, 65</t>
+    <t>eyes_closed_start</t>
+  </si>
+  <si>
+    <t>eyes_closed_stop</t>
+  </si>
+  <si>
+    <t>eyes_open_start</t>
+  </si>
+  <si>
+    <t>eyes_open_stop</t>
+  </si>
+  <si>
+    <t>9500, 126750</t>
+  </si>
+  <si>
+    <t>86500, 210500</t>
+  </si>
+  <si>
+    <t>234000</t>
+  </si>
+  <si>
+    <t>309750</t>
   </si>
 </sst>
 </file>
@@ -567,15 +507,17 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3"/>
     <col min="2" max="2" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -583,13 +525,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>23</v>
@@ -598,35 +540,35 @@
         <v>24</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5">
         <v>0</v>
@@ -634,23 +576,19 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="6">
-        <v>3.9009999999999998</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
       <c r="G4" s="10">
         <v>25</v>
       </c>
@@ -660,145 +598,97 @@
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="10" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="10" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="10" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>
@@ -806,26 +696,19 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="10">
         <v>25</v>
       </c>
@@ -835,33 +718,25 @@
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B13" s="4">
         <v>1</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="10" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B14" s="5">
         <v>0</v>
@@ -869,26 +744,19 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="10">
         <v>25</v>
       </c>
@@ -898,7 +766,7 @@
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B16" s="5">
         <v>0</v>
@@ -906,10 +774,11 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B17" s="5">
         <v>0</v>
@@ -917,6 +786,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D17" xr:uid="{D3E9F8EE-C051-614B-878A-6F3E56936703}"/>

</xml_diff>